<commit_message>
Updating results and RC3 code bug fixes
</commit_message>
<xml_diff>
--- a/goldendata/Assigment3_E2/BitcountAndPSNRGraphsExercise2.xlsx
+++ b/goldendata/Assigment3_E2/BitcountAndPSNRGraphsExercise2.xlsx
@@ -9,17 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RD - GRAPHS" sheetId="1" r:id="rId1"/>
     <sheet name="RawData" sheetId="2" r:id="rId2"/>
     <sheet name="PSNR-GRAPHS" sheetId="4" r:id="rId3"/>
-    <sheet name="Constant qp BitCount" sheetId="6" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,15 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
-  <si>
-    <t>Costant Qp</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>Frame</t>
-  </si>
-  <si>
-    <t>Rate control</t>
   </si>
   <si>
     <t>Constant QP</t>
@@ -69,6 +59,12 @@
   </si>
   <si>
     <t>bps</t>
+  </si>
+  <si>
+    <t>RC3</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -344,10 +340,10 @@
                   <c:v>13302.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79718.428571428565</c:v>
+                  <c:v>81560.71428571429</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>213346.71428571429</c:v>
+                  <c:v>220630.19047619047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,10 +358,10 @@
                   <c:v>21.517742619047617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.841372333333332</c:v>
+                  <c:v>32.426199238095236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.380713714285704</c:v>
+                  <c:v>39.548047523809529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,13 +418,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21828.476190476191</c:v>
+                  <c:v>11943.190476190477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76768.619047619053</c:v>
+                  <c:v>68767.952380952382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>184917.04761904763</c:v>
+                  <c:v>190142.23809523811</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,13 +436,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26.247897952380953</c:v>
+                  <c:v>19.713755666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.168051952380956</c:v>
+                  <c:v>36.651466285714285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.159323190476186</c:v>
+                  <c:v>42.458324285714284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,6 +451,87 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0CA1-440D-A08A-E2AA7D88F8EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'RD - GRAPHS'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RC3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'RD - GRAPHS'!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12336.761904761905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72504.333333333328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205275.71428571429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'RD - GRAPHS'!$I$2:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>19.96633404761905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.766081714285718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.651430333333323</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6533-4AC0-983A-21A9195C23B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -929,64 +1006,64 @@
                   <c:v>32.922676000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.755074</c:v>
+                  <c:v>34.446255000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.083424000000001</c:v>
+                  <c:v>34.772243000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.199699000000003</c:v>
+                  <c:v>35.180957999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.044659000000003</c:v>
+                  <c:v>35.254860000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.590591000000003</c:v>
+                  <c:v>35.075470000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.923457999999997</c:v>
+                  <c:v>35.319267000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.799461000000001</c:v>
+                  <c:v>20.453419</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.378185000000002</c:v>
+                  <c:v>28.630528999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.091048999999998</c:v>
+                  <c:v>33.728476999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.734969999999997</c:v>
+                  <c:v>35.681579999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.058281000000001</c:v>
+                  <c:v>36.381531000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.224747000000001</c:v>
+                  <c:v>36.802371999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.193446999999999</c:v>
+                  <c:v>37.012076999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.674053000000001</c:v>
+                  <c:v>20.808565000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32.070366</c:v>
+                  <c:v>25.208953999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32.523223999999999</c:v>
+                  <c:v>31.867751999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.397342999999999</c:v>
+                  <c:v>32.325004999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.81382</c:v>
+                  <c:v>32.867843999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.603405000000002</c:v>
+                  <c:v>33.129677000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.586886999999997</c:v>
+                  <c:v>33.080672999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,67 +1120,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>30.367435</c:v>
+                  <c:v>31.998732</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.918883999999998</c:v>
+                  <c:v>33.66404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.631259999999997</c:v>
+                  <c:v>34.269011999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.500602999999998</c:v>
+                  <c:v>33.985416000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.389885</c:v>
+                  <c:v>34.765396000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.704239000000001</c:v>
+                  <c:v>34.167797</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.220275999999998</c:v>
+                  <c:v>35.411414999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.440894999999998</c:v>
+                  <c:v>37.519649999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.930701999999997</c:v>
+                  <c:v>39.888767000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.279502999999998</c:v>
+                  <c:v>42.570678999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41.126185999999997</c:v>
+                  <c:v>43.398173999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.311821000000002</c:v>
+                  <c:v>43.061348000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.268920999999999</c:v>
+                  <c:v>44.530689000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46.669379999999997</c:v>
+                  <c:v>44.044246999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>32.999721999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.886490000000002</c:v>
+                  <c:v>34.283462999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.959510999999999</c:v>
+                  <c:v>34.402926999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.696449000000001</c:v>
+                  <c:v>33.734946999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33.051009999999998</c:v>
+                  <c:v>34.009940999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.556015000000002</c:v>
+                  <c:v>34.118617999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.619903999999998</c:v>
+                  <c:v>32.855812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1163,6 +1240,123 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6A2C-4216-BE11-04657B9942C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'PSNR-GRAPHS'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RC3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'PSNR-GRAPHS'!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>33.625340000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.232193000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.240195999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.036437999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.891540999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.121532000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.506691000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.519649999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.839129999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40.97636</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.372535999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.893104999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.424343</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43.893970000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.999721999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34.054993000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34.033225999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.989097999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33.959816000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33.829993999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33.647841999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2891-4261-828E-AF1C450B0C52}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1412,608 +1606,10 @@
           <c:yMode val="edge"/>
           <c:x val="0.25405457651126945"/>
           <c:y val="0.88175623496818645"/>
-          <c:w val="0.52575328083989503"/>
-          <c:h val="6.9103700046979716E-2"/>
+          <c:w val="0.35234312377619464"/>
+          <c:h val="6.6333031970556622E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>CIF Bitcount per Frame with I_Period 21</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>RateControl</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Constant qp BitCount'!$P$3:$P$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>81524</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>83325</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>81810</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>81089</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>82940</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80535</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85019</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>85675</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>81952</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>82766</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>82222</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>78872</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80207</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>71573</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>83747</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>82772</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>88240</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>86108</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>80786</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>81640</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>80726</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C7DA-46B0-B3A4-E291B99D355C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>QP-4</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Constant qp BitCount'!$E$3:$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>141254</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>105334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>98473</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>91715</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>97724</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>97256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>81433</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>215548</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>62364</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>46443</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>40788</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40053</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39462</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>37070</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>219219</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>122341</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>116305</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>112679</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>116700</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>117471</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>120901</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C7DA-46B0-B3A4-E291B99D355C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="373196216"/>
-        <c:axId val="373193864"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="373196216"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Frame</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="373193864"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="373193864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Bitcount</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="373196216"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2121,46 +1717,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3219,522 +2775,19 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3769,16 +2822,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>139065</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>131444</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>169544</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3806,147 +2859,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>140969</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>150495</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE3E938-8689-4F50-883F-C57EE6C3B466}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Block 8"/>
-      <sheetName val="Block 16"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="A4">
-            <v>4263450</v>
-          </cell>
-          <cell r="B4">
-            <v>37.906968200000001</v>
-          </cell>
-          <cell r="C4">
-            <v>3744411</v>
-          </cell>
-          <cell r="D4">
-            <v>38.142766599999995</v>
-          </cell>
-          <cell r="E4">
-            <v>3651043</v>
-          </cell>
-          <cell r="F4">
-            <v>37.690782999999996</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>1254681</v>
-          </cell>
-          <cell r="B5">
-            <v>31.191080400000004</v>
-          </cell>
-          <cell r="C5">
-            <v>905625</v>
-          </cell>
-          <cell r="D5">
-            <v>31.409247700000002</v>
-          </cell>
-          <cell r="E5">
-            <v>807006</v>
-          </cell>
-          <cell r="F5">
-            <v>31.530800699999997</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>202445</v>
-          </cell>
-          <cell r="B6">
-            <v>26.649968999999999</v>
-          </cell>
-          <cell r="C6">
-            <v>164799</v>
-          </cell>
-          <cell r="D6">
-            <v>27.544206999999993</v>
-          </cell>
-          <cell r="E6">
-            <v>149099</v>
-          </cell>
-          <cell r="F6">
-            <v>27.967571499999998</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>38717</v>
-          </cell>
-          <cell r="B7">
-            <v>18.360233200000003</v>
-          </cell>
-          <cell r="C7">
-            <v>77027</v>
-          </cell>
-          <cell r="D7">
-            <v>19.3384827</v>
-          </cell>
-          <cell r="E7">
-            <v>87034</v>
-          </cell>
-          <cell r="F7">
-            <v>19.818847399999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4246,10 +3158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,18 +3169,21 @@
     <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="H1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -4285,13 +3200,19 @@
         <v>21.517742619047617</v>
       </c>
       <c r="F2">
-        <v>21828.476190476191</v>
+        <v>11943.190476190477</v>
       </c>
       <c r="G2">
-        <v>26.247897952380953</v>
+        <v>19.713755666666671</v>
+      </c>
+      <c r="H2">
+        <v>12336.761904761905</v>
+      </c>
+      <c r="I2">
+        <v>19.96633404761905</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -4302,19 +3223,34 @@
         <v>27.994726428571425</v>
       </c>
       <c r="D3">
-        <v>79718.428571428565</v>
+        <v>81560.71428571429</v>
       </c>
       <c r="E3">
-        <v>33.841372333333332</v>
+        <v>32.426199238095236</v>
       </c>
       <c r="F3">
+        <v>68767.952380952382</v>
+      </c>
+      <c r="G3">
+        <v>36.651466285714285</v>
+      </c>
+      <c r="H3">
+        <v>72504.333333333328</v>
+      </c>
+      <c r="I3">
+        <v>36.766081714285718</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3">
         <v>76768.619047619053</v>
       </c>
-      <c r="G3">
+      <c r="M3">
         <v>36.168051952380956</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4325,19 +3261,25 @@
         <v>36.352430523809524</v>
       </c>
       <c r="D4">
-        <v>213346.71428571429</v>
+        <v>220630.19047619047</v>
       </c>
       <c r="E4">
-        <v>40.380713714285704</v>
+        <v>39.548047523809529</v>
       </c>
       <c r="F4">
-        <v>184917.04761904763</v>
+        <v>190142.23809523811</v>
       </c>
       <c r="G4">
-        <v>42.159323190476186</v>
+        <v>42.458324285714284</v>
+      </c>
+      <c r="H4">
+        <v>205275.71428571429</v>
+      </c>
+      <c r="I4">
+        <v>42.651430333333323</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4348,7 +3290,7 @@
         <v>38.988259857142857</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4359,12 +3301,12 @@
         <v>41.812136714285721</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4375,7 +3317,7 @@
         <v>19.136953714285717</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4386,7 +3328,7 @@
         <v>21.303869142857145</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -4397,7 +3339,7 @@
         <v>25.610374857142865</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -4408,7 +3350,7 @@
         <v>27.994726428571425</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -4419,7 +3361,7 @@
         <v>36.352430523809524</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4430,7 +3372,7 @@
         <v>38.988259857142857</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -4441,29 +3383,32 @@
         <v>41.812136714285721</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -4474,13 +3419,16 @@
         <v>7000000</v>
       </c>
       <c r="D19">
-        <v>106.02</v>
+        <v>124.86</v>
       </c>
       <c r="E19">
-        <v>220.56</v>
+        <v>237.83</v>
+      </c>
+      <c r="F19">
+        <v>175.63</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -4491,13 +3439,16 @@
         <v>2400000</v>
       </c>
       <c r="D20">
-        <v>119.25</v>
+        <v>123.6</v>
       </c>
       <c r="E20">
-        <v>235.02</v>
+        <v>242.44</v>
+      </c>
+      <c r="F20">
+        <v>167.39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -4508,13 +3459,16 @@
         <v>36000</v>
       </c>
       <c r="D21">
-        <v>113.93</v>
+        <v>110.27</v>
       </c>
       <c r="E21">
-        <v>236.18</v>
+        <v>233.97</v>
+      </c>
+      <c r="F21">
+        <v>217.85</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4522,7 +3476,7 @@
         <v>112.18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -4538,10 +3492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ23"/>
+  <dimension ref="A1:AQ23"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2:AH22"/>
+      <selection activeCell="AO2" sqref="AO2:AO22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4550,12 +3504,12 @@
     <col min="3" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -4588,31 +3542,43 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" t="s">
         <v>4</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>8</v>
-      </c>
       <c r="AD1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>8</v>
+      <c r="AK1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4689,31 +3655,49 @@
         <v>32.922676000000003</v>
       </c>
       <c r="AB2">
-        <v>239492</v>
+        <v>237225</v>
       </c>
       <c r="AC2">
-        <v>39.864452</v>
+        <v>39.829174000000002</v>
       </c>
       <c r="AE2">
-        <v>13621</v>
+        <v>12686</v>
       </c>
       <c r="AF2">
-        <v>18.321864999999999</v>
+        <v>19.131360999999998</v>
       </c>
       <c r="AG2">
-        <v>59615</v>
+        <v>70733</v>
       </c>
       <c r="AH2">
-        <v>30.367435</v>
+        <v>31.998732</v>
       </c>
       <c r="AI2">
-        <v>174891</v>
+        <v>217757</v>
       </c>
       <c r="AJ2">
-        <v>37.327744000000003</v>
+        <v>39.163272999999997</v>
+      </c>
+      <c r="AL2">
+        <v>20951</v>
+      </c>
+      <c r="AM2">
+        <v>24.435507000000001</v>
+      </c>
+      <c r="AN2">
+        <v>84229</v>
+      </c>
+      <c r="AO2">
+        <v>33.625340000000001</v>
+      </c>
+      <c r="AP2">
+        <v>102758</v>
+      </c>
+      <c r="AQ2">
+        <v>34.102176999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4784,37 +3768,55 @@
         <v>22.573967</v>
       </c>
       <c r="Z3">
-        <v>79355</v>
+        <v>79430</v>
       </c>
       <c r="AA3">
-        <v>34.755074</v>
+        <v>34.446255000000001</v>
       </c>
       <c r="AB3">
-        <v>238881</v>
+        <v>231621</v>
       </c>
       <c r="AC3">
-        <v>40.929690999999998</v>
+        <v>40.867767000000001</v>
       </c>
       <c r="AE3">
-        <v>7108</v>
+        <v>12369</v>
       </c>
       <c r="AF3">
-        <v>21.794861000000001</v>
+        <v>19.387526000000001</v>
       </c>
       <c r="AG3">
-        <v>68844</v>
+        <v>63386</v>
       </c>
       <c r="AH3">
-        <v>33.918883999999998</v>
+        <v>33.66404</v>
       </c>
       <c r="AI3">
-        <v>188152</v>
+        <v>181238</v>
       </c>
       <c r="AJ3">
-        <v>39.991734000000001</v>
+        <v>39.900351999999998</v>
+      </c>
+      <c r="AL3">
+        <v>12369</v>
+      </c>
+      <c r="AM3">
+        <v>19.387526000000001</v>
+      </c>
+      <c r="AN3">
+        <v>64658</v>
+      </c>
+      <c r="AO3">
+        <v>34.232193000000002</v>
+      </c>
+      <c r="AP3">
+        <v>211922</v>
+      </c>
+      <c r="AQ3">
+        <v>39.397129</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4885,37 +3887,55 @@
         <v>22.485600000000002</v>
       </c>
       <c r="Z4">
-        <v>80385</v>
+        <v>83005</v>
       </c>
       <c r="AA4">
-        <v>35.083424000000001</v>
+        <v>34.772243000000003</v>
       </c>
       <c r="AB4">
-        <v>233275</v>
+        <v>233004</v>
       </c>
       <c r="AC4">
-        <v>40.641810999999997</v>
+        <v>41.006207000000003</v>
       </c>
       <c r="AE4">
-        <v>7179</v>
+        <v>12575</v>
       </c>
       <c r="AF4">
-        <v>22.131240999999999</v>
+        <v>19.797535</v>
       </c>
       <c r="AG4">
-        <v>74572</v>
+        <v>66294</v>
       </c>
       <c r="AH4">
-        <v>34.631259999999997</v>
+        <v>34.269011999999996</v>
       </c>
       <c r="AI4">
-        <v>193732</v>
+        <v>198078</v>
       </c>
       <c r="AJ4">
-        <v>40.277107000000001</v>
+        <v>40.414073999999999</v>
+      </c>
+      <c r="AL4">
+        <v>12575</v>
+      </c>
+      <c r="AM4">
+        <v>19.797535</v>
+      </c>
+      <c r="AN4">
+        <v>55577</v>
+      </c>
+      <c r="AO4">
+        <v>34.240195999999997</v>
+      </c>
+      <c r="AP4">
+        <v>177753</v>
+      </c>
+      <c r="AQ4">
+        <v>39.768462999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4986,37 +4006,55 @@
         <v>22.433809</v>
       </c>
       <c r="Z5">
-        <v>75914</v>
+        <v>80234</v>
       </c>
       <c r="AA5">
-        <v>35.199699000000003</v>
+        <v>35.180957999999997</v>
       </c>
       <c r="AB5">
-        <v>234785</v>
+        <v>236484</v>
       </c>
       <c r="AC5">
-        <v>41.214767000000002</v>
+        <v>41.843105000000001</v>
       </c>
       <c r="AE5">
-        <v>37563</v>
+        <v>11925</v>
       </c>
       <c r="AF5">
-        <v>27.276586999999999</v>
+        <v>19.552675000000001</v>
       </c>
       <c r="AG5">
-        <v>42831</v>
+        <v>46146</v>
       </c>
       <c r="AH5">
-        <v>34.500602999999998</v>
+        <v>33.985416000000001</v>
       </c>
       <c r="AI5">
-        <v>196493</v>
+        <v>163846</v>
       </c>
       <c r="AJ5">
-        <v>40.677055000000003</v>
+        <v>40.103157000000003</v>
+      </c>
+      <c r="AL5">
+        <v>11925</v>
+      </c>
+      <c r="AM5">
+        <v>19.552675000000001</v>
+      </c>
+      <c r="AN5">
+        <v>110073</v>
+      </c>
+      <c r="AO5">
+        <v>36.036437999999997</v>
+      </c>
+      <c r="AP5">
+        <v>235467</v>
+      </c>
+      <c r="AQ5">
+        <v>41.285418999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5087,37 +4125,55 @@
         <v>22.457798</v>
       </c>
       <c r="Z6">
-        <v>78739</v>
+        <v>80568</v>
       </c>
       <c r="AA6">
-        <v>35.044659000000003</v>
+        <v>35.254860000000001</v>
       </c>
       <c r="AB6">
-        <v>234766</v>
+        <v>237525</v>
       </c>
       <c r="AC6">
-        <v>40.747967000000003</v>
+        <v>41.549281999999998</v>
       </c>
       <c r="AE6">
-        <v>24423</v>
+        <v>12478</v>
       </c>
       <c r="AF6">
-        <v>28.924848999999998</v>
+        <v>19.048214000000002</v>
       </c>
       <c r="AG6">
-        <v>47883</v>
+        <v>71076</v>
       </c>
       <c r="AH6">
-        <v>33.389885</v>
+        <v>34.765396000000003</v>
       </c>
       <c r="AI6">
-        <v>173021</v>
+        <v>171986</v>
       </c>
       <c r="AJ6">
-        <v>39.966124999999998</v>
+        <v>39.873997000000003</v>
+      </c>
+      <c r="AL6">
+        <v>12478</v>
+      </c>
+      <c r="AM6">
+        <v>19.048214000000002</v>
+      </c>
+      <c r="AN6">
+        <v>52927</v>
+      </c>
+      <c r="AO6">
+        <v>34.891540999999997</v>
+      </c>
+      <c r="AP6">
+        <v>237655</v>
+      </c>
+      <c r="AQ6">
+        <v>41.569350999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5188,37 +4244,55 @@
         <v>22.425180000000001</v>
       </c>
       <c r="Z7">
-        <v>82386</v>
+        <v>80301</v>
       </c>
       <c r="AA7">
-        <v>34.590591000000003</v>
+        <v>35.075470000000003</v>
       </c>
       <c r="AB7">
-        <v>230567</v>
+        <v>234496</v>
       </c>
       <c r="AC7">
-        <v>40.536278000000003</v>
+        <v>41.149731000000003</v>
       </c>
       <c r="AE7">
-        <v>20708</v>
+        <v>11881</v>
       </c>
       <c r="AF7">
-        <v>27.292387000000002</v>
+        <v>18.731864999999999</v>
       </c>
       <c r="AG7">
-        <v>72702</v>
+        <v>48845</v>
       </c>
       <c r="AH7">
-        <v>33.704239000000001</v>
+        <v>34.167797</v>
       </c>
       <c r="AI7">
-        <v>173175</v>
+        <v>196930</v>
       </c>
       <c r="AJ7">
-        <v>39.5914</v>
+        <v>40.276733</v>
+      </c>
+      <c r="AL7">
+        <v>11881</v>
+      </c>
+      <c r="AM7">
+        <v>18.731864999999999</v>
+      </c>
+      <c r="AN7">
+        <v>105039</v>
+      </c>
+      <c r="AO7">
+        <v>36.121532000000002</v>
+      </c>
+      <c r="AP7">
+        <v>247648</v>
+      </c>
+      <c r="AQ7">
+        <v>41.458221000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5289,37 +4363,55 @@
         <v>22.261185000000001</v>
       </c>
       <c r="Z8">
-        <v>80236</v>
+        <v>78053</v>
       </c>
       <c r="AA8">
-        <v>34.923457999999997</v>
+        <v>35.319267000000004</v>
       </c>
       <c r="AB8">
-        <v>225121</v>
+        <v>232739</v>
       </c>
       <c r="AC8">
-        <v>41.280974999999998</v>
+        <v>42.175593999999997</v>
       </c>
       <c r="AE8">
-        <v>50483</v>
+        <v>12134</v>
       </c>
       <c r="AF8">
-        <v>30.784282999999999</v>
+        <v>18.125368000000002</v>
       </c>
       <c r="AG8">
-        <v>88142</v>
+        <v>86866</v>
       </c>
       <c r="AH8">
-        <v>35.220275999999998</v>
+        <v>35.411414999999998</v>
       </c>
       <c r="AI8">
-        <v>168772</v>
+        <v>173943</v>
       </c>
       <c r="AJ8">
-        <v>40.468418</v>
+        <v>40.782494</v>
+      </c>
+      <c r="AL8">
+        <v>12134</v>
+      </c>
+      <c r="AM8">
+        <v>18.125368000000002</v>
+      </c>
+      <c r="AN8">
+        <v>53573</v>
+      </c>
+      <c r="AO8">
+        <v>35.506691000000004</v>
+      </c>
+      <c r="AP8">
+        <v>211075</v>
+      </c>
+      <c r="AQ8">
+        <v>41.958126</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5390,16 +4482,16 @@
         <v>21.718384</v>
       </c>
       <c r="Z9">
-        <v>81368</v>
+        <v>85362</v>
       </c>
       <c r="AA9">
-        <v>30.799461000000001</v>
+        <v>20.453419</v>
       </c>
       <c r="AB9">
-        <v>241149</v>
+        <v>235185</v>
       </c>
       <c r="AC9">
-        <v>38.162227999999999</v>
+        <v>24.518744000000002</v>
       </c>
       <c r="AE9">
         <v>11589</v>
@@ -5408,19 +4500,37 @@
         <v>22.001522000000001</v>
       </c>
       <c r="AG9">
-        <v>74878</v>
+        <v>77495</v>
       </c>
       <c r="AH9">
-        <v>37.440894999999998</v>
+        <v>37.519649999999999</v>
       </c>
       <c r="AI9">
-        <v>211685</v>
+        <v>213105</v>
       </c>
       <c r="AJ9">
-        <v>44.857757999999997</v>
+        <v>45.155082999999998</v>
+      </c>
+      <c r="AL9">
+        <v>11589</v>
+      </c>
+      <c r="AM9">
+        <v>22.001522000000001</v>
+      </c>
+      <c r="AN9">
+        <v>77495</v>
+      </c>
+      <c r="AO9">
+        <v>37.519649999999999</v>
+      </c>
+      <c r="AP9">
+        <v>213105</v>
+      </c>
+      <c r="AQ9">
+        <v>45.155082999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5491,37 +4601,55 @@
         <v>21.973611999999999</v>
       </c>
       <c r="Z10">
-        <v>80704</v>
+        <v>80910</v>
       </c>
       <c r="AA10">
-        <v>33.378185000000002</v>
+        <v>28.630528999999999</v>
       </c>
       <c r="AB10">
-        <v>227200</v>
+        <v>239145</v>
       </c>
       <c r="AC10">
-        <v>41.439109999999999</v>
+        <v>39.853630000000003</v>
       </c>
       <c r="AE10">
-        <v>5266</v>
+        <v>11385</v>
       </c>
       <c r="AF10">
-        <v>24.328092999999999</v>
+        <v>21.999476999999999</v>
       </c>
       <c r="AG10">
-        <v>62875</v>
+        <v>65374</v>
       </c>
       <c r="AH10">
-        <v>38.930701999999997</v>
+        <v>39.888767000000001</v>
       </c>
       <c r="AI10">
-        <v>203479</v>
+        <v>238461</v>
       </c>
       <c r="AJ10">
-        <v>47.393822</v>
+        <v>47.835735</v>
+      </c>
+      <c r="AL10">
+        <v>11385</v>
+      </c>
+      <c r="AM10">
+        <v>21.999476999999999</v>
+      </c>
+      <c r="AN10">
+        <v>65089</v>
+      </c>
+      <c r="AO10">
+        <v>39.839129999999997</v>
+      </c>
+      <c r="AP10">
+        <v>183551</v>
+      </c>
+      <c r="AQ10">
+        <v>47.141219999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5592,37 +4720,55 @@
         <v>21.847237</v>
       </c>
       <c r="Z11">
-        <v>84128</v>
+        <v>81750</v>
       </c>
       <c r="AA11">
-        <v>35.091048999999998</v>
+        <v>33.728476999999998</v>
       </c>
       <c r="AB11">
-        <v>184535</v>
+        <v>235747</v>
       </c>
       <c r="AC11">
-        <v>42.280166999999999</v>
+        <v>42.332458000000003</v>
       </c>
       <c r="AE11">
-        <v>44707</v>
+        <v>11575</v>
       </c>
       <c r="AF11">
-        <v>32.850231000000001</v>
+        <v>21.995365</v>
       </c>
       <c r="AG11">
-        <v>78761</v>
+        <v>110922</v>
       </c>
       <c r="AH11">
-        <v>40.279502999999998</v>
+        <v>42.570678999999998</v>
       </c>
       <c r="AI11">
-        <v>173866</v>
+        <v>182897</v>
       </c>
       <c r="AJ11">
-        <v>47.811069000000003</v>
+        <v>48.042301000000002</v>
+      </c>
+      <c r="AL11">
+        <v>11575</v>
+      </c>
+      <c r="AM11">
+        <v>21.995365</v>
+      </c>
+      <c r="AN11">
+        <v>64017</v>
+      </c>
+      <c r="AO11">
+        <v>40.97636</v>
+      </c>
+      <c r="AP11">
+        <v>197804</v>
+      </c>
+      <c r="AQ11">
+        <v>47.837657999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5693,37 +4839,55 @@
         <v>22.064775000000001</v>
       </c>
       <c r="Z12">
-        <v>77388</v>
+        <v>82954</v>
       </c>
       <c r="AA12">
-        <v>35.734969999999997</v>
+        <v>35.681579999999997</v>
       </c>
       <c r="AB12">
-        <v>152539</v>
+        <v>171164</v>
       </c>
       <c r="AC12">
-        <v>42.493267000000003</v>
+        <v>42.655025000000002</v>
       </c>
       <c r="AE12">
-        <v>9246</v>
+        <v>11342</v>
       </c>
       <c r="AF12">
-        <v>31.192207</v>
+        <v>21.929424000000001</v>
       </c>
       <c r="AG12">
-        <v>101840</v>
+        <v>82331</v>
       </c>
       <c r="AH12">
-        <v>41.126185999999997</v>
+        <v>43.398173999999997</v>
       </c>
       <c r="AI12">
-        <v>166375</v>
+        <v>168112</v>
       </c>
       <c r="AJ12">
-        <v>47.984386000000001</v>
+        <v>48.149951999999999</v>
+      </c>
+      <c r="AL12">
+        <v>11342</v>
+      </c>
+      <c r="AM12">
+        <v>21.929424000000001</v>
+      </c>
+      <c r="AN12">
+        <v>81173</v>
+      </c>
+      <c r="AO12">
+        <v>42.372535999999997</v>
+      </c>
+      <c r="AP12">
+        <v>178317</v>
+      </c>
+      <c r="AQ12">
+        <v>48.076309000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5794,37 +4958,55 @@
         <v>22.267133999999999</v>
       </c>
       <c r="Z13">
-        <v>70651</v>
+        <v>78899</v>
       </c>
       <c r="AA13">
-        <v>36.058281000000001</v>
+        <v>36.381531000000003</v>
       </c>
       <c r="AB13">
-        <v>131986</v>
+        <v>156934</v>
       </c>
       <c r="AC13">
-        <v>42.687859000000003</v>
+        <v>42.909153000000003</v>
       </c>
       <c r="AE13">
-        <v>53647</v>
+        <v>11559</v>
       </c>
       <c r="AF13">
-        <v>35.207023999999997</v>
+        <v>22.00441</v>
       </c>
       <c r="AG13">
-        <v>104473</v>
+        <v>29879</v>
       </c>
       <c r="AH13">
-        <v>42.311821000000002</v>
+        <v>43.061348000000002</v>
       </c>
       <c r="AI13">
-        <v>159396</v>
+        <v>167428</v>
       </c>
       <c r="AJ13">
-        <v>48.006686999999999</v>
+        <v>48.157443999999998</v>
+      </c>
+      <c r="AL13">
+        <v>11559</v>
+      </c>
+      <c r="AM13">
+        <v>22.00441</v>
+      </c>
+      <c r="AN13">
+        <v>68635</v>
+      </c>
+      <c r="AO13">
+        <v>42.893104999999998</v>
+      </c>
+      <c r="AP13">
+        <v>170728</v>
+      </c>
+      <c r="AQ13">
+        <v>48.119762000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5895,37 +5077,55 @@
         <v>22.283674000000001</v>
       </c>
       <c r="Z14">
-        <v>72614</v>
+        <v>77323</v>
       </c>
       <c r="AA14">
-        <v>36.224747000000001</v>
+        <v>36.802371999999998</v>
       </c>
       <c r="AB14">
-        <v>123965</v>
+        <v>144270</v>
       </c>
       <c r="AC14">
-        <v>42.849421999999997</v>
+        <v>42.972408000000001</v>
       </c>
       <c r="AE14">
-        <v>27764</v>
+        <v>11342</v>
       </c>
       <c r="AF14">
-        <v>30.445623000000001</v>
+        <v>21.959574</v>
       </c>
       <c r="AG14">
-        <v>123532</v>
+        <v>121636</v>
       </c>
       <c r="AH14">
-        <v>45.268920999999999</v>
+        <v>44.530689000000002</v>
       </c>
       <c r="AI14">
-        <v>154253</v>
+        <v>162264</v>
       </c>
       <c r="AJ14">
-        <v>48.018566</v>
+        <v>48.190978999999999</v>
+      </c>
+      <c r="AL14">
+        <v>11342</v>
+      </c>
+      <c r="AM14">
+        <v>21.959574</v>
+      </c>
+      <c r="AN14">
+        <v>75102</v>
+      </c>
+      <c r="AO14">
+        <v>43.424343</v>
+      </c>
+      <c r="AP14">
+        <v>163487</v>
+      </c>
+      <c r="AQ14">
+        <v>48.160075999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5996,37 +5196,55 @@
         <v>22.356574999999999</v>
       </c>
       <c r="Z15">
-        <v>66604</v>
+        <v>77122</v>
       </c>
       <c r="AA15">
-        <v>36.193446999999999</v>
+        <v>37.012076999999998</v>
       </c>
       <c r="AB15">
-        <v>118492</v>
+        <v>136890</v>
       </c>
       <c r="AC15">
-        <v>42.856335000000001</v>
+        <v>42.982033000000001</v>
       </c>
       <c r="AE15">
-        <v>30218</v>
+        <v>11386</v>
       </c>
       <c r="AF15">
-        <v>34.456992999999997</v>
+        <v>22.026772000000001</v>
       </c>
       <c r="AG15">
-        <v>131350</v>
+        <v>36603</v>
       </c>
       <c r="AH15">
-        <v>46.669379999999997</v>
+        <v>44.044246999999999</v>
       </c>
       <c r="AI15">
-        <v>153694</v>
+        <v>160099</v>
       </c>
       <c r="AJ15">
-        <v>48.019069999999999</v>
+        <v>48.182819000000002</v>
+      </c>
+      <c r="AL15">
+        <v>11386</v>
+      </c>
+      <c r="AM15">
+        <v>22.026772000000001</v>
+      </c>
+      <c r="AN15">
+        <v>111965</v>
+      </c>
+      <c r="AO15">
+        <v>43.893970000000003</v>
+      </c>
+      <c r="AP15">
+        <v>161717</v>
+      </c>
+      <c r="AQ15">
+        <v>48.153824</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -6097,16 +5315,16 @@
         <v>19.781756999999999</v>
       </c>
       <c r="Z16">
-        <v>81588</v>
+        <v>84442</v>
       </c>
       <c r="AA16">
-        <v>29.674053000000001</v>
+        <v>20.808565000000002</v>
       </c>
       <c r="AB16">
-        <v>239474</v>
+        <v>234608</v>
       </c>
       <c r="AC16">
-        <v>36.940193000000001</v>
+        <v>29.096529</v>
       </c>
       <c r="AE16">
         <v>12233</v>
@@ -6121,13 +5339,31 @@
         <v>32.999721999999998</v>
       </c>
       <c r="AI16">
-        <v>233705</v>
+        <v>238683</v>
       </c>
       <c r="AJ16">
-        <v>39.681648000000003</v>
+        <v>39.744903999999998</v>
+      </c>
+      <c r="AL16">
+        <v>12233</v>
+      </c>
+      <c r="AM16">
+        <v>17.986937999999999</v>
+      </c>
+      <c r="AN16">
+        <v>83187</v>
+      </c>
+      <c r="AO16">
+        <v>32.999721999999998</v>
+      </c>
+      <c r="AP16">
+        <v>238683</v>
+      </c>
+      <c r="AQ16">
+        <v>39.744903999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -6198,37 +5434,55 @@
         <v>20.325771</v>
       </c>
       <c r="Z17">
-        <v>83447</v>
+        <v>81715</v>
       </c>
       <c r="AA17">
-        <v>32.070366</v>
+        <v>25.208953999999999</v>
       </c>
       <c r="AB17">
-        <v>235495</v>
+        <v>242663</v>
       </c>
       <c r="AC17">
-        <v>38.729202000000001</v>
+        <v>38.327057000000003</v>
       </c>
       <c r="AE17">
-        <v>6735</v>
+        <v>12365</v>
       </c>
       <c r="AF17">
-        <v>20.739386</v>
+        <v>19.018329999999999</v>
       </c>
       <c r="AG17">
-        <v>72229</v>
+        <v>75219</v>
       </c>
       <c r="AH17">
-        <v>33.886490000000002</v>
+        <v>34.283462999999998</v>
       </c>
       <c r="AI17">
-        <v>185645</v>
+        <v>198212</v>
       </c>
       <c r="AJ17">
-        <v>40.286808000000001</v>
+        <v>40.328831000000001</v>
+      </c>
+      <c r="AL17">
+        <v>12365</v>
+      </c>
+      <c r="AM17">
+        <v>19.018329999999999</v>
+      </c>
+      <c r="AN17">
+        <v>65418</v>
+      </c>
+      <c r="AO17">
+        <v>34.054993000000003</v>
+      </c>
+      <c r="AP17">
+        <v>245000</v>
+      </c>
+      <c r="AQ17">
+        <v>41.388458</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -6299,37 +5553,55 @@
         <v>20.644192</v>
       </c>
       <c r="Z18">
-        <v>84603</v>
+        <v>84323</v>
       </c>
       <c r="AA18">
-        <v>32.523223999999999</v>
+        <v>31.867751999999999</v>
       </c>
       <c r="AB18">
-        <v>234828</v>
+        <v>237410</v>
       </c>
       <c r="AC18">
-        <v>39.018044000000003</v>
+        <v>39.124831999999998</v>
       </c>
       <c r="AE18">
-        <v>5598</v>
+        <v>11633</v>
       </c>
       <c r="AF18">
-        <v>21.812218000000001</v>
+        <v>17.842775</v>
       </c>
       <c r="AG18">
-        <v>72311</v>
+        <v>68519</v>
       </c>
       <c r="AH18">
-        <v>33.959510999999999</v>
+        <v>34.402926999999998</v>
       </c>
       <c r="AI18">
-        <v>202071</v>
+        <v>196005</v>
       </c>
       <c r="AJ18">
-        <v>39.660156000000001</v>
+        <v>39.779201999999998</v>
+      </c>
+      <c r="AL18">
+        <v>11633</v>
+      </c>
+      <c r="AM18">
+        <v>17.842775</v>
+      </c>
+      <c r="AN18">
+        <v>61722</v>
+      </c>
+      <c r="AO18">
+        <v>34.033225999999999</v>
+      </c>
+      <c r="AP18">
+        <v>254877</v>
+      </c>
+      <c r="AQ18">
+        <v>41.285881000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -6400,37 +5672,55 @@
         <v>20.80517</v>
       </c>
       <c r="Z19">
-        <v>79536</v>
+        <v>81268</v>
       </c>
       <c r="AA19">
-        <v>32.397342999999999</v>
+        <v>32.325004999999997</v>
       </c>
       <c r="AB19">
-        <v>236954</v>
+        <v>237798</v>
       </c>
       <c r="AC19">
-        <v>38.815891000000001</v>
+        <v>39.259520999999999</v>
       </c>
       <c r="AE19">
-        <v>31544</v>
+        <v>12260</v>
       </c>
       <c r="AF19">
-        <v>25.874516</v>
+        <v>17.986751999999999</v>
       </c>
       <c r="AG19">
-        <v>51900</v>
+        <v>53929</v>
       </c>
       <c r="AH19">
-        <v>32.696449000000001</v>
+        <v>33.734946999999998</v>
       </c>
       <c r="AI19">
-        <v>193524</v>
+        <v>190367</v>
       </c>
       <c r="AJ19">
-        <v>39.107384000000003</v>
+        <v>39.727921000000002</v>
+      </c>
+      <c r="AL19">
+        <v>12260</v>
+      </c>
+      <c r="AM19">
+        <v>17.986751999999999</v>
+      </c>
+      <c r="AN19">
+        <v>58137</v>
+      </c>
+      <c r="AO19">
+        <v>33.989097999999998</v>
+      </c>
+      <c r="AP19">
+        <v>249275</v>
+      </c>
+      <c r="AQ19">
+        <v>41.246276999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -6501,37 +5791,55 @@
         <v>20.688877000000002</v>
       </c>
       <c r="Z20">
-        <v>85019</v>
+        <v>83736</v>
       </c>
       <c r="AA20">
-        <v>32.81382</v>
+        <v>32.867843999999998</v>
       </c>
       <c r="AB20">
-        <v>237500</v>
+        <v>241014</v>
       </c>
       <c r="AC20">
-        <v>38.957946999999997</v>
+        <v>39.657803000000001</v>
       </c>
       <c r="AE20">
-        <v>14738</v>
+        <v>12106</v>
       </c>
       <c r="AF20">
-        <v>25.931823999999999</v>
+        <v>17.934822</v>
       </c>
       <c r="AG20">
-        <v>73809</v>
+        <v>67031</v>
       </c>
       <c r="AH20">
-        <v>33.051009999999998</v>
+        <v>34.009940999999998</v>
       </c>
       <c r="AI20">
-        <v>193819</v>
+        <v>188336</v>
       </c>
       <c r="AJ20">
-        <v>39.018146999999999</v>
+        <v>39.487659000000001</v>
+      </c>
+      <c r="AL20">
+        <v>12106</v>
+      </c>
+      <c r="AM20">
+        <v>17.934822</v>
+      </c>
+      <c r="AN20">
+        <v>59117</v>
+      </c>
+      <c r="AO20">
+        <v>33.959816000000004</v>
+      </c>
+      <c r="AP20">
+        <v>250904</v>
+      </c>
+      <c r="AQ20">
+        <v>41.207904999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -6602,37 +5910,55 @@
         <v>20.813203999999999</v>
       </c>
       <c r="Z21">
-        <v>83885</v>
+        <v>86368</v>
       </c>
       <c r="AA21">
-        <v>32.603405000000002</v>
+        <v>33.129677000000001</v>
       </c>
       <c r="AB21">
-        <v>238947</v>
+        <v>238698</v>
       </c>
       <c r="AC21">
-        <v>38.757354999999997</v>
+        <v>39.31559</v>
       </c>
       <c r="AE21">
-        <v>40670</v>
+        <v>12073</v>
       </c>
       <c r="AF21">
-        <v>28.398903000000001</v>
+        <v>17.749901000000001</v>
       </c>
       <c r="AG21">
-        <v>62040</v>
+        <v>69067</v>
       </c>
       <c r="AH21">
-        <v>32.556015000000002</v>
+        <v>34.118617999999998</v>
       </c>
       <c r="AI21">
-        <v>200297</v>
+        <v>199786</v>
       </c>
       <c r="AJ21">
-        <v>39.001914999999997</v>
+        <v>39.504879000000003</v>
+      </c>
+      <c r="AL21">
+        <v>12073</v>
+      </c>
+      <c r="AM21">
+        <v>17.749901000000001</v>
+      </c>
+      <c r="AN21">
+        <v>60714</v>
+      </c>
+      <c r="AO21">
+        <v>33.829993999999999</v>
+      </c>
+      <c r="AP21">
+        <v>186190</v>
+      </c>
+      <c r="AQ21">
+        <v>39.451557000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -6703,37 +6029,55 @@
         <v>20.881637999999999</v>
       </c>
       <c r="Z22">
-        <v>84160</v>
+        <v>83635</v>
       </c>
       <c r="AA22">
-        <v>32.586886999999997</v>
+        <v>33.080672999999997</v>
       </c>
       <c r="AB22">
-        <v>240330</v>
+        <v>238614</v>
       </c>
       <c r="AC22">
-        <v>38.792026999999997</v>
+        <v>39.083354999999997</v>
       </c>
       <c r="AE22">
-        <v>3358</v>
+        <v>11911</v>
       </c>
       <c r="AF22">
-        <v>23.454305999999999</v>
+        <v>17.778262999999999</v>
       </c>
       <c r="AG22">
-        <v>64367</v>
+        <v>49589</v>
       </c>
       <c r="AH22">
-        <v>32.619903999999998</v>
+        <v>32.855812</v>
       </c>
       <c r="AI22">
-        <v>183213</v>
+        <v>185454</v>
       </c>
       <c r="AJ22">
-        <v>38.198788</v>
+        <v>38.823020999999997</v>
+      </c>
+      <c r="AL22">
+        <v>11911</v>
+      </c>
+      <c r="AM22">
+        <v>17.778262999999999</v>
+      </c>
+      <c r="AN22">
+        <v>64744</v>
+      </c>
+      <c r="AO22">
+        <v>33.647841999999997</v>
+      </c>
+      <c r="AP22">
+        <v>192874</v>
+      </c>
+      <c r="AQ22">
+        <v>39.172237000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C23">
         <f>AVERAGE(C2:C22)</f>
         <v>311008.38095238095</v>
@@ -6763,7 +6107,7 @@
         <v>100977.76190476191</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:AJ23" si="1">AVERAGE(J2:J22)</f>
+        <f t="shared" ref="J23:AQ23" si="1">AVERAGE(J2:J22)</f>
         <v>36.352430523809524</v>
       </c>
       <c r="K23">
@@ -6828,47 +6172,67 @@
       </c>
       <c r="Z23">
         <f t="shared" si="1"/>
-        <v>79718.428571428565</v>
+        <v>81560.71428571429</v>
       </c>
       <c r="AA23">
         <f t="shared" si="1"/>
-        <v>33.841372333333332</v>
+        <v>32.426199238095236</v>
       </c>
       <c r="AB23">
         <f t="shared" si="1"/>
-        <v>213346.71428571429</v>
+        <v>220630.19047619047</v>
       </c>
       <c r="AC23">
         <f t="shared" si="1"/>
-        <v>40.380713714285704</v>
-      </c>
-      <c r="AD23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>39.548047523809529</v>
       </c>
       <c r="AE23">
         <f t="shared" si="1"/>
-        <v>21828.476190476191</v>
+        <v>11943.190476190477</v>
       </c>
       <c r="AF23">
         <f t="shared" si="1"/>
-        <v>26.247897952380953</v>
+        <v>19.713755666666671</v>
       </c>
       <c r="AG23">
         <f t="shared" si="1"/>
-        <v>76768.619047619053</v>
+        <v>68767.952380952382</v>
       </c>
       <c r="AH23">
         <f t="shared" si="1"/>
-        <v>36.168051952380956</v>
+        <v>36.651466285714285</v>
       </c>
       <c r="AI23">
         <f t="shared" si="1"/>
-        <v>184917.04761904763</v>
+        <v>190142.23809523811</v>
       </c>
       <c r="AJ23">
         <f t="shared" si="1"/>
-        <v>42.159323190476186</v>
+        <v>42.458324285714284</v>
+      </c>
+      <c r="AL23">
+        <f t="shared" si="1"/>
+        <v>12336.761904761905</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="1"/>
+        <v>19.96633404761905</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="1"/>
+        <v>72504.333333333328</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="1"/>
+        <v>36.766081714285718</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="1"/>
+        <v>205275.71428571429</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="1"/>
+        <v>42.651430333333323</v>
       </c>
     </row>
   </sheetData>
@@ -6878,26 +6242,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6905,637 +6272,290 @@
         <v>32.922676000000003</v>
       </c>
       <c r="C2">
-        <v>30.367435</v>
+        <v>31.998732</v>
+      </c>
+      <c r="D2">
+        <v>33.625340000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>34.755074</v>
+        <v>34.446255000000001</v>
       </c>
       <c r="C3">
-        <v>33.918883999999998</v>
+        <v>33.66404</v>
+      </c>
+      <c r="D3">
+        <v>34.232193000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>35.083424000000001</v>
+        <v>34.772243000000003</v>
       </c>
       <c r="C4">
-        <v>34.631259999999997</v>
+        <v>34.269011999999996</v>
+      </c>
+      <c r="D4">
+        <v>34.240195999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>35.199699000000003</v>
+        <v>35.180957999999997</v>
       </c>
       <c r="C5">
-        <v>34.500602999999998</v>
+        <v>33.985416000000001</v>
+      </c>
+      <c r="D5">
+        <v>36.036437999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>35.044659000000003</v>
+        <v>35.254860000000001</v>
       </c>
       <c r="C6">
-        <v>33.389885</v>
+        <v>34.765396000000003</v>
+      </c>
+      <c r="D6">
+        <v>34.891540999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>34.590591000000003</v>
+        <v>35.075470000000003</v>
       </c>
       <c r="C7">
-        <v>33.704239000000001</v>
+        <v>34.167797</v>
+      </c>
+      <c r="D7">
+        <v>36.121532000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>34.923457999999997</v>
+        <v>35.319267000000004</v>
       </c>
       <c r="C8">
-        <v>35.220275999999998</v>
+        <v>35.411414999999998</v>
+      </c>
+      <c r="D8">
+        <v>35.506691000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>30.799461000000001</v>
+        <v>20.453419</v>
       </c>
       <c r="C9">
-        <v>37.440894999999998</v>
+        <v>37.519649999999999</v>
+      </c>
+      <c r="D9">
+        <v>37.519649999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>33.378185000000002</v>
+        <v>28.630528999999999</v>
       </c>
       <c r="C10">
-        <v>38.930701999999997</v>
+        <v>39.888767000000001</v>
+      </c>
+      <c r="D10">
+        <v>39.839129999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>35.091048999999998</v>
+        <v>33.728476999999998</v>
       </c>
       <c r="C11">
-        <v>40.279502999999998</v>
+        <v>42.570678999999998</v>
+      </c>
+      <c r="D11">
+        <v>40.97636</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>35.734969999999997</v>
+        <v>35.681579999999997</v>
       </c>
       <c r="C12">
-        <v>41.126185999999997</v>
+        <v>43.398173999999997</v>
+      </c>
+      <c r="D12">
+        <v>42.372535999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>36.058281000000001</v>
+        <v>36.381531000000003</v>
       </c>
       <c r="C13">
-        <v>42.311821000000002</v>
+        <v>43.061348000000002</v>
+      </c>
+      <c r="D13">
+        <v>42.893104999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>36.224747000000001</v>
+        <v>36.802371999999998</v>
       </c>
       <c r="C14">
-        <v>45.268920999999999</v>
+        <v>44.530689000000002</v>
+      </c>
+      <c r="D14">
+        <v>43.424343</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>36.193446999999999</v>
+        <v>37.012076999999998</v>
       </c>
       <c r="C15">
-        <v>46.669379999999997</v>
+        <v>44.044246999999999</v>
+      </c>
+      <c r="D15">
+        <v>43.893970000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>29.674053000000001</v>
+        <v>20.808565000000002</v>
       </c>
       <c r="C16">
         <v>32.999721999999998</v>
       </c>
+      <c r="D16">
+        <v>32.999721999999998</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>32.070366</v>
+        <v>25.208953999999999</v>
       </c>
       <c r="C17">
-        <v>33.886490000000002</v>
+        <v>34.283462999999998</v>
+      </c>
+      <c r="D17">
+        <v>34.054993000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>32.523223999999999</v>
+        <v>31.867751999999999</v>
       </c>
       <c r="C18">
-        <v>33.959510999999999</v>
+        <v>34.402926999999998</v>
+      </c>
+      <c r="D18">
+        <v>34.033225999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>32.397342999999999</v>
+        <v>32.325004999999997</v>
       </c>
       <c r="C19">
-        <v>32.696449000000001</v>
+        <v>33.734946999999998</v>
+      </c>
+      <c r="D19">
+        <v>33.989097999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>32.81382</v>
+        <v>32.867843999999998</v>
       </c>
       <c r="C20">
-        <v>33.051009999999998</v>
+        <v>34.009940999999998</v>
+      </c>
+      <c r="D20">
+        <v>33.959816000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>32.603405000000002</v>
+        <v>33.129677000000001</v>
       </c>
       <c r="C21">
-        <v>32.556015000000002</v>
+        <v>34.118617999999998</v>
+      </c>
+      <c r="D21">
+        <v>33.829993999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>32.586886999999997</v>
+        <v>33.080672999999997</v>
       </c>
       <c r="C22">
-        <v>32.619903999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
-  <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>11</v>
-      </c>
-      <c r="N2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>141254</v>
-      </c>
-      <c r="F3">
-        <v>83903</v>
-      </c>
-      <c r="P3">
-        <v>81524</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>105334</v>
-      </c>
-      <c r="F4">
-        <v>59482</v>
-      </c>
-      <c r="P4">
-        <v>83325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>98473</v>
-      </c>
-      <c r="F5">
-        <v>53449</v>
-      </c>
-      <c r="P5">
-        <v>81810</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>91715</v>
-      </c>
-      <c r="F6">
-        <v>47518</v>
-      </c>
-      <c r="P6">
-        <v>81089</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>97724</v>
-      </c>
-      <c r="F7">
-        <v>50026</v>
-      </c>
-      <c r="P7">
-        <v>82940</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>97256</v>
-      </c>
-      <c r="F8">
-        <v>52165</v>
-      </c>
-      <c r="P8">
-        <v>80535</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>81433</v>
-      </c>
-      <c r="F9">
-        <v>45079</v>
-      </c>
-      <c r="P9">
-        <v>85019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>215548</v>
-      </c>
-      <c r="F10">
-        <v>144573</v>
-      </c>
-      <c r="P10">
-        <v>85675</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>62364</v>
-      </c>
-      <c r="F11">
-        <v>40597</v>
-      </c>
-      <c r="P11">
-        <v>81952</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>46443</v>
-      </c>
-      <c r="F12">
-        <v>33020</v>
-      </c>
-      <c r="P12">
-        <v>82766</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>40788</v>
-      </c>
-      <c r="F13">
-        <v>31159</v>
-      </c>
-      <c r="P13">
-        <v>82222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="E14">
-        <v>40053</v>
-      </c>
-      <c r="F14">
-        <v>30320</v>
-      </c>
-      <c r="P14">
-        <v>78872</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="E15">
-        <v>39462</v>
-      </c>
-      <c r="F15">
-        <v>30151</v>
-      </c>
-      <c r="P15">
-        <v>80207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="E16">
-        <v>37070</v>
-      </c>
-      <c r="F16">
-        <v>29050</v>
-      </c>
-      <c r="P16">
-        <v>71573</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="E17">
-        <v>219219</v>
-      </c>
-      <c r="F17">
-        <v>144110</v>
-      </c>
-      <c r="P17">
-        <v>83747</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="E18">
-        <v>122341</v>
-      </c>
-      <c r="F18">
-        <v>68919</v>
-      </c>
-      <c r="P18">
-        <v>82772</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="E19">
-        <v>116305</v>
-      </c>
-      <c r="F19">
-        <v>62691</v>
-      </c>
-      <c r="P19">
-        <v>88240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="E20">
-        <v>112679</v>
-      </c>
-      <c r="F20">
-        <v>62883</v>
-      </c>
-      <c r="P20">
-        <v>86108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="E21">
-        <v>116700</v>
-      </c>
-      <c r="F21">
-        <v>60007</v>
-      </c>
-      <c r="P21">
-        <v>80786</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="E22">
-        <v>117471</v>
-      </c>
-      <c r="F22">
-        <v>64820</v>
-      </c>
-      <c r="P22">
-        <v>81640</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="E23">
-        <v>120901</v>
-      </c>
-      <c r="F23">
-        <v>66290</v>
-      </c>
-      <c r="P23">
-        <v>80726</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <f>SUM(E2:E23)</f>
-        <v>2120536</v>
-      </c>
-      <c r="F24">
-        <f>SUM(F3:F23)</f>
-        <v>1260212</v>
-      </c>
-      <c r="J24">
-        <f t="shared" ref="J24:P24" si="0">SUM(J3:J23)</f>
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>1723528</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E25">
-        <f>P24/E24</f>
-        <v>0.81277941048866886</v>
-      </c>
-      <c r="F25">
-        <f>P24/F24</f>
-        <v>1.3676492526654245</v>
+        <v>32.855812</v>
+      </c>
+      <c r="D22">
+        <v>33.647841999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>